<commit_message>
feat: update end point search
</commit_message>
<xml_diff>
--- a/src/scape/diadiem - Copy.xlsx
+++ b/src/scape/diadiem - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HOCKY8\DO_AN_TOT_NGHIEP\dev\ScapeData\model_cursor\src\scape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C46CE59-C537-491D-B441-003852AC1230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35FF60D-5019-43B8-9937-F8EAE516DA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5D481351-B047-447E-A56F-CECAC2589BFC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="1304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="1306">
   <si>
     <t>id</t>
   </si>
@@ -3951,13 +3951,19 @@
   </si>
   <si>
     <t>https://cdn.tgdd.vn/Files/2021/06/25/1363265/top-6-dia-diem-du-lich-vui-choi-cuc-chat-tai-cu-chi-202202161137511543.jpg</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3973,6 +3979,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3982,7 +3993,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -3990,14 +4001,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4333,19 +4362,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB04EF8-036A-4785-AF66-860F6DCB82E1}">
-  <dimension ref="A1:K224"/>
+  <dimension ref="A1:M224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4376,8 +4407,14 @@
       <c r="J1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L1" s="2" t="s">
+        <v>1304</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4408,8 +4445,14 @@
       <c r="J2">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>10.776994199999979</v>
+      </c>
+      <c r="M2">
+        <v>106.69530210000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4440,8 +4483,14 @@
       <c r="J3">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>10.77251680000002</v>
+      </c>
+      <c r="M3">
+        <v>106.69802079999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4472,8 +4521,14 @@
       <c r="J4">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>10.770035900000019</v>
+      </c>
+      <c r="M4">
+        <v>106.6991736999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4504,8 +4559,14 @@
       <c r="J5">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>10.77384950000002</v>
+      </c>
+      <c r="M5">
+        <v>106.7036566</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4536,8 +4597,14 @@
       <c r="J6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>10.767125400000021</v>
+      </c>
+      <c r="M6">
+        <v>106.6931448</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4568,8 +4635,14 @@
       <c r="J7">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>10.779785499999999</v>
+      </c>
+      <c r="M7">
+        <v>106.6990189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4600,8 +4673,14 @@
       <c r="J8">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>10.775702699999989</v>
+      </c>
+      <c r="M8">
+        <v>106.7069595</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4632,8 +4711,14 @@
       <c r="J9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>10.78096299999998</v>
+      </c>
+      <c r="M9">
+        <v>106.70007339999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4664,8 +4749,14 @@
       <c r="J10">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>10.77797159999999</v>
+      </c>
+      <c r="M10">
+        <v>106.70165040000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4696,8 +4787,14 @@
       <c r="J11">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>10.853019999999971</v>
+      </c>
+      <c r="M11">
+        <v>106.79340000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4728,8 +4825,14 @@
       <c r="J12">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>10.773408699999999</v>
+      </c>
+      <c r="M12">
+        <v>106.7038889</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4760,8 +4863,14 @@
       <c r="J13">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>10.76871139999999</v>
+      </c>
+      <c r="M13">
+        <v>106.69234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4792,8 +4901,14 @@
       <c r="J14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>10.80556910000001</v>
+      </c>
+      <c r="M14">
+        <v>106.73802499999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4824,8 +4939,14 @@
       <c r="J15">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>10.81691070000001</v>
+      </c>
+      <c r="M15">
+        <v>106.72976319999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4856,8 +4977,14 @@
       <c r="J16">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>10.802379599999981</v>
+      </c>
+      <c r="M16">
+        <v>106.74097159999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4888,8 +5015,14 @@
       <c r="J17">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>10.772177799999991</v>
+      </c>
+      <c r="M17">
+        <v>106.7246327</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4920,8 +5053,14 @@
       <c r="J18">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>10.77034730000001</v>
+      </c>
+      <c r="M18">
+        <v>106.7098527</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4952,8 +5091,14 @@
       <c r="J19">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>10.778752199999991</v>
+      </c>
+      <c r="M19">
+        <v>106.746685</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4984,8 +5129,14 @@
       <c r="J20">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>10.804528800000019</v>
+      </c>
+      <c r="M20">
+        <v>106.7394266</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5016,8 +5167,14 @@
       <c r="J21">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>10.780561400000011</v>
+      </c>
+      <c r="M21">
+        <v>106.6807936</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5048,8 +5205,14 @@
       <c r="J22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <v>10.78514779999999</v>
+      </c>
+      <c r="M22">
+        <v>106.6647487</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5080,8 +5243,14 @@
       <c r="J23">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>10.7826608</v>
+      </c>
+      <c r="M23">
+        <v>106.695915</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5112,8 +5281,14 @@
       <c r="J24">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>10.788335899999989</v>
+      </c>
+      <c r="M24">
+        <v>106.69067889999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5144,8 +5319,14 @@
       <c r="J25">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>10.778021200000021</v>
+      </c>
+      <c r="M25">
+        <v>106.68690460000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5176,8 +5357,14 @@
       <c r="J26">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <v>10.76951460000002</v>
+      </c>
+      <c r="M26">
+        <v>106.6838554</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5208,8 +5395,14 @@
       <c r="J27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <v>10.782044500000019</v>
+      </c>
+      <c r="M27">
+        <v>106.68168780000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5240,8 +5433,14 @@
       <c r="J28">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L28">
+        <v>10.77109500000001</v>
+      </c>
+      <c r="M28">
+        <v>106.68602629999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5272,8 +5471,14 @@
       <c r="J29">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <v>10.780761999999999</v>
+      </c>
+      <c r="M29">
+        <v>106.6899808</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5304,8 +5509,14 @@
       <c r="J30">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <v>10.76811049999999</v>
+      </c>
+      <c r="M30">
+        <v>106.703653</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5336,8 +5547,14 @@
       <c r="J31">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <v>10.768166600000001</v>
+      </c>
+      <c r="M31">
+        <v>106.70686619999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5368,8 +5585,14 @@
       <c r="J32">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L32">
+        <v>10.763563499999989</v>
+      </c>
+      <c r="M32">
+        <v>106.7060311</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5400,8 +5623,14 @@
       <c r="J33">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <v>10.758098699999991</v>
+      </c>
+      <c r="M33">
+        <v>106.698859</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5432,8 +5661,14 @@
       <c r="J34">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <v>10.75723210000003</v>
+      </c>
+      <c r="M34">
+        <v>106.6985583</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5464,8 +5699,14 @@
       <c r="J35">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <v>21.03839940000001</v>
+      </c>
+      <c r="M35">
+        <v>105.84674769999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5496,8 +5737,14 @@
       <c r="J36">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <v>10.766954200000001</v>
+      </c>
+      <c r="M36">
+        <v>106.7082494</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5528,8 +5775,14 @@
       <c r="J37">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <v>10.7613933</v>
+      </c>
+      <c r="M37">
+        <v>106.7026953</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5560,8 +5813,14 @@
       <c r="J38">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L38">
+        <v>10.752437200000021</v>
+      </c>
+      <c r="M38">
+        <v>106.6679015</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5592,8 +5851,14 @@
       <c r="J39">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <v>10.7530336</v>
+      </c>
+      <c r="M39">
+        <v>106.6599837</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5624,8 +5889,14 @@
       <c r="J40">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <v>10.753749300000029</v>
+      </c>
+      <c r="M40">
+        <v>106.65745099999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5656,8 +5927,14 @@
       <c r="J41">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L41">
+        <v>10.7645959</v>
+      </c>
+      <c r="M41">
+        <v>106.6557035</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5688,8 +5965,14 @@
       <c r="J42">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L42">
+        <v>10.753258300000009</v>
+      </c>
+      <c r="M42">
+        <v>106.6611736</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5720,8 +6003,14 @@
       <c r="J43">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L43">
+        <v>10.754648899999999</v>
+      </c>
+      <c r="M43">
+        <v>106.6569997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5752,8 +6041,14 @@
       <c r="J44">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L44">
+        <v>10.7581989</v>
+      </c>
+      <c r="M44">
+        <v>106.6722817</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5784,8 +6079,14 @@
       <c r="J45">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L45">
+        <v>10.76578150000001</v>
+      </c>
+      <c r="M45">
+        <v>106.69069</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5816,8 +6117,14 @@
       <c r="J46">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L46">
+        <v>10.752437200000021</v>
+      </c>
+      <c r="M46">
+        <v>106.6679015</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5848,8 +6155,14 @@
       <c r="J47">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L47">
+        <v>10.74936469999999</v>
+      </c>
+      <c r="M47">
+        <v>106.65105800000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5880,8 +6193,14 @@
       <c r="J48">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L48">
+        <v>10.75410819999999</v>
+      </c>
+      <c r="M48">
+        <v>106.6406618</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5912,8 +6231,14 @@
       <c r="J49">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L49">
+        <v>10.787099799999989</v>
+      </c>
+      <c r="M49">
+        <v>106.6595018</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5944,8 +6269,14 @@
       <c r="J50">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L50">
+        <v>10.741554199999991</v>
+      </c>
+      <c r="M50">
+        <v>106.6950038999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5976,8 +6307,14 @@
       <c r="J51">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L51">
+        <v>10.705174</v>
+      </c>
+      <c r="M51">
+        <v>106.7269785</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6008,8 +6345,14 @@
       <c r="J52">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L52">
+        <v>10.730232100000009</v>
+      </c>
+      <c r="M52">
+        <v>106.70339749999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6040,8 +6383,14 @@
       <c r="J53">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L53">
+        <v>10.728535200000019</v>
+      </c>
+      <c r="M53">
+        <v>106.71874680000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -6072,8 +6421,14 @@
       <c r="J54">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L54">
+        <v>10.74216</v>
+      </c>
+      <c r="M54">
+        <v>106.6952009</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -6104,8 +6459,14 @@
       <c r="J55">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L55">
+        <v>10.770446800000011</v>
+      </c>
+      <c r="M55">
+        <v>106.6699412</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -6136,8 +6497,14 @@
       <c r="J56">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L56">
+        <v>10.741925599999989</v>
+      </c>
+      <c r="M56">
+        <v>106.7158003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6168,8 +6535,14 @@
       <c r="J57">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L57">
+        <v>10.72315850000003</v>
+      </c>
+      <c r="M57">
+        <v>106.7265963</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6200,8 +6573,14 @@
       <c r="J58">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L58">
+        <v>10.72471950000001</v>
+      </c>
+      <c r="M58">
+        <v>106.71857900000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -6232,8 +6611,14 @@
       <c r="J59">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L59">
+        <v>10.744608499999989</v>
+      </c>
+      <c r="M59">
+        <v>106.7443687</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -6264,8 +6649,14 @@
       <c r="J60">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L60">
+        <v>10.743128499999999</v>
+      </c>
+      <c r="M60">
+        <v>106.7347262</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -6296,8 +6687,14 @@
       <c r="J61">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L61">
+        <v>10.70227390000001</v>
+      </c>
+      <c r="M61">
+        <v>106.6086365</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6328,8 +6725,14 @@
       <c r="J62">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L62">
+        <v>10.74323319999999</v>
+      </c>
+      <c r="M62">
+        <v>106.6506181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -6360,8 +6763,14 @@
       <c r="J63">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L63">
+        <v>10.86171980000001</v>
+      </c>
+      <c r="M63">
+        <v>106.801727</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6392,8 +6801,14 @@
       <c r="J64">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L64">
+        <v>10.845001400000021</v>
+      </c>
+      <c r="M64">
+        <v>106.7802104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6424,8 +6839,14 @@
       <c r="J65">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L65">
+        <v>10.74751630000002</v>
+      </c>
+      <c r="M65">
+        <v>106.6689121</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -6456,8 +6877,14 @@
       <c r="J66">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L66">
+        <v>10.73677570000002</v>
+      </c>
+      <c r="M66">
+        <v>106.669023</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6488,8 +6915,14 @@
       <c r="J67">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L67">
+        <v>10.734203600000001</v>
+      </c>
+      <c r="M67">
+        <v>106.6532521</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6520,8 +6953,14 @@
       <c r="J68">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L68">
+        <v>10.73478849999999</v>
+      </c>
+      <c r="M68">
+        <v>106.6403361</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6552,8 +6991,14 @@
       <c r="J69">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L69">
+        <v>10.736962800000001</v>
+      </c>
+      <c r="M69">
+        <v>106.65708309999999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6584,8 +7029,14 @@
       <c r="J70">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L70">
+        <v>10.820377000000001</v>
+      </c>
+      <c r="M70">
+        <v>106.7787964</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6616,8 +7067,14 @@
       <c r="J71">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L71">
+        <v>10.74359430000001</v>
+      </c>
+      <c r="M71">
+        <v>106.6540794</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6648,8 +7105,14 @@
       <c r="J72">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L72">
+        <v>10.90800609999998</v>
+      </c>
+      <c r="M72">
+        <v>106.7532193</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6680,8 +7143,14 @@
       <c r="J73">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L73">
+        <v>10.74943400000001</v>
+      </c>
+      <c r="M73">
+        <v>106.685608</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6712,8 +7181,14 @@
       <c r="J74">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L74">
+        <v>10.83962949999999</v>
+      </c>
+      <c r="M74">
+        <v>106.8456912</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6744,8 +7219,14 @@
       <c r="J75">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L75">
+        <v>10.80863840000001</v>
+      </c>
+      <c r="M75">
+        <v>106.87722650000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6776,8 +7257,14 @@
       <c r="J76">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L76">
+        <v>10.8088861</v>
+      </c>
+      <c r="M76">
+        <v>106.8532216</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6808,8 +7295,14 @@
       <c r="J77">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L77">
+        <v>10.79447529999997</v>
+      </c>
+      <c r="M77">
+        <v>106.84295899999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6840,8 +7333,14 @@
       <c r="J78">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L78">
+        <v>10.87885769999998</v>
+      </c>
+      <c r="M78">
+        <v>106.83498040000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6872,8 +7371,14 @@
       <c r="J79">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L79">
+        <v>10.888889000000001</v>
+      </c>
+      <c r="M79">
+        <v>106.8243827</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6904,8 +7409,14 @@
       <c r="J80">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L80">
+        <v>10.85372390000002</v>
+      </c>
+      <c r="M80">
+        <v>106.8140509</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6936,8 +7447,14 @@
       <c r="J81">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L81">
+        <v>10.87942329999998</v>
+      </c>
+      <c r="M81">
+        <v>106.8458953</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6968,8 +7485,14 @@
       <c r="J82">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L82">
+        <v>10.843301499999979</v>
+      </c>
+      <c r="M82">
+        <v>106.8425105</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -7000,8 +7523,14 @@
       <c r="J83">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L83">
+        <v>10.8206229</v>
+      </c>
+      <c r="M83">
+        <v>106.86905609999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -7032,8 +7561,14 @@
       <c r="J84">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L84">
+        <v>10.78672820000002</v>
+      </c>
+      <c r="M84">
+        <v>106.7938441</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -7064,8 +7599,14 @@
       <c r="J85">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L85">
+        <v>10.833701899999991</v>
+      </c>
+      <c r="M85">
+        <v>106.86043530000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -7096,8 +7637,14 @@
       <c r="J86">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L86">
+        <v>10.77084629999997</v>
+      </c>
+      <c r="M86">
+        <v>106.6696383</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -7128,8 +7675,14 @@
       <c r="J87">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L87">
+        <v>10.785501500000001</v>
+      </c>
+      <c r="M87">
+        <v>106.66605300000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -7160,8 +7713,14 @@
       <c r="J88">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L88">
+        <v>10.760941600000001</v>
+      </c>
+      <c r="M88">
+        <v>106.66015470000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -7192,8 +7751,14 @@
       <c r="J89">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L89">
+        <v>10.776188400000009</v>
+      </c>
+      <c r="M89">
+        <v>106.6718953</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -7224,8 +7789,14 @@
       <c r="J90">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L90">
+        <v>10.77212780000001</v>
+      </c>
+      <c r="M90">
+        <v>106.6733505</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -7256,8 +7827,14 @@
       <c r="J91">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L91">
+        <v>10.77229510000002</v>
+      </c>
+      <c r="M91">
+        <v>106.67392150000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -7288,8 +7865,14 @@
       <c r="J92">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L92">
+        <v>10.76515950000003</v>
+      </c>
+      <c r="M92">
+        <v>106.6770144</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -7320,8 +7903,14 @@
       <c r="J93">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L93">
+        <v>10.78514779999999</v>
+      </c>
+      <c r="M93">
+        <v>106.6647487</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -7352,8 +7941,14 @@
       <c r="J94">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L94">
+        <v>10.77614899999999</v>
+      </c>
+      <c r="M94">
+        <v>106.6806398999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -7384,8 +7979,14 @@
       <c r="J95">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L95">
+        <v>10.866119000000021</v>
+      </c>
+      <c r="M95">
+        <v>106.8029346</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -7416,8 +8017,14 @@
       <c r="J96">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L96">
+        <v>10.843810600000021</v>
+      </c>
+      <c r="M96">
+        <v>106.76428009999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -7448,8 +8055,14 @@
       <c r="J97">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L97">
+        <v>10.763617800000009</v>
+      </c>
+      <c r="M97">
+        <v>106.66786930000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -7480,8 +8093,14 @@
       <c r="J98">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L98">
+        <v>10.7634603</v>
+      </c>
+      <c r="M98">
+        <v>106.6672397</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -7512,8 +8131,14 @@
       <c r="J99">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L99">
+        <v>10.762983999999999</v>
+      </c>
+      <c r="M99">
+        <v>106.67396669999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -7544,8 +8169,14 @@
       <c r="J100">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L100">
+        <v>10.777233600000001</v>
+      </c>
+      <c r="M100">
+        <v>106.6651292</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -7576,8 +8207,14 @@
       <c r="J101">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L101">
+        <v>10.76609799999998</v>
+      </c>
+      <c r="M101">
+        <v>106.6418936</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -7608,8 +8245,14 @@
       <c r="J102">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L102">
+        <v>10.763118600000031</v>
+      </c>
+      <c r="M102">
+        <v>106.65671469999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -7640,8 +8283,14 @@
       <c r="J103">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L103">
+        <v>10.76452950000002</v>
+      </c>
+      <c r="M103">
+        <v>106.6557487</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -7672,8 +8321,14 @@
       <c r="J104">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L104">
+        <v>10.76902850000001</v>
+      </c>
+      <c r="M104">
+        <v>106.6577739</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -7704,8 +8359,14 @@
       <c r="J105">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L105">
+        <v>10.764612099999979</v>
+      </c>
+      <c r="M105">
+        <v>106.6587593</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -7736,8 +8397,14 @@
       <c r="J106">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L106">
+        <v>10.827294200000029</v>
+      </c>
+      <c r="M106">
+        <v>106.76951939999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -7768,8 +8435,14 @@
       <c r="J107">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L107">
+        <v>10.850553299999991</v>
+      </c>
+      <c r="M107">
+        <v>106.76703910000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -7800,8 +8473,14 @@
       <c r="J108">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L108">
+        <v>10.85614820000001</v>
+      </c>
+      <c r="M108">
+        <v>106.76647850000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -7832,8 +8511,14 @@
       <c r="J109">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L109">
+        <v>10.879736499999989</v>
+      </c>
+      <c r="M109">
+        <v>106.81126620000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -7864,8 +8549,14 @@
       <c r="J110">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L110">
+        <v>10.7635912</v>
+      </c>
+      <c r="M110">
+        <v>106.6544383</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -7896,8 +8587,14 @@
       <c r="J111">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L111">
+        <v>10.772164000000011</v>
+      </c>
+      <c r="M111">
+        <v>106.6563618</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -7928,8 +8625,14 @@
       <c r="J112">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L112">
+        <v>10.758157799999999</v>
+      </c>
+      <c r="M112">
+        <v>106.65262250000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -7960,8 +8663,14 @@
       <c r="J113">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L113">
+        <v>10.761435599999979</v>
+      </c>
+      <c r="M113">
+        <v>106.6583091</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -7992,8 +8701,14 @@
       <c r="J114">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L114">
+        <v>10.7951119</v>
+      </c>
+      <c r="M114">
+        <v>106.72209599999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -8024,8 +8739,14 @@
       <c r="J115">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L115">
+        <v>10.793430799999999</v>
+      </c>
+      <c r="M115">
+        <v>106.7243981</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -8056,8 +8777,14 @@
       <c r="J116">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L116">
+        <v>10.7740446</v>
+      </c>
+      <c r="M116">
+        <v>106.70409650000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -8088,8 +8815,14 @@
       <c r="J117">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L117">
+        <v>10.79817869999999</v>
+      </c>
+      <c r="M117">
+        <v>106.7157267</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -8120,8 +8853,14 @@
       <c r="J118">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L118">
+        <v>10.79996420000001</v>
+      </c>
+      <c r="M118">
+        <v>106.7247441</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -8152,8 +8891,14 @@
       <c r="J119">
         <v>4</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L119">
+        <v>10.833402400000031</v>
+      </c>
+      <c r="M119">
+        <v>106.7436933</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -8184,8 +8929,14 @@
       <c r="J120">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L120">
+        <v>10.833402400000031</v>
+      </c>
+      <c r="M120">
+        <v>106.7436933</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -8216,8 +8967,14 @@
       <c r="J121">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L121">
+        <v>10.801881000000011</v>
+      </c>
+      <c r="M121">
+        <v>106.696907</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -8248,8 +9005,14 @@
       <c r="J122">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L122">
+        <v>10.801604700000009</v>
+      </c>
+      <c r="M122">
+        <v>106.69881719999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -8280,8 +9043,14 @@
       <c r="J123">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L123">
+        <v>10.79724049999998</v>
+      </c>
+      <c r="M123">
+        <v>106.7178717</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -8312,8 +9081,14 @@
       <c r="J124">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L124">
+        <v>10.79663740000001</v>
+      </c>
+      <c r="M124">
+        <v>106.69341609999999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -8344,8 +9119,14 @@
       <c r="J125">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L125">
+        <v>10.832186200000001</v>
+      </c>
+      <c r="M125">
+        <v>106.7048973</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -8376,8 +9157,14 @@
       <c r="J126">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L126">
+        <v>10.82370359999998</v>
+      </c>
+      <c r="M126">
+        <v>106.7317099</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -8408,8 +9195,14 @@
       <c r="J127">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L127">
+        <v>10.80582489999999</v>
+      </c>
+      <c r="M127">
+        <v>106.71347919999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -8440,8 +9233,14 @@
       <c r="J128">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L128">
+        <v>10.85307980000001</v>
+      </c>
+      <c r="M128">
+        <v>106.6779009</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -8472,8 +9271,14 @@
       <c r="J129">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L129">
+        <v>10.86108189999999</v>
+      </c>
+      <c r="M129">
+        <v>106.7050888</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -8504,8 +9309,14 @@
       <c r="J130">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L130">
+        <v>10.87499070000001</v>
+      </c>
+      <c r="M130">
+        <v>106.6828275</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -8536,8 +9347,14 @@
       <c r="J131">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L131">
+        <v>10.895885</v>
+      </c>
+      <c r="M131">
+        <v>106.680488</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -8568,8 +9385,14 @@
       <c r="J132">
         <v>4</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L132">
+        <v>10.853739600000001</v>
+      </c>
+      <c r="M132">
+        <v>106.6255914</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -8600,8 +9423,14 @@
       <c r="J133">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L133">
+        <v>10.8569847</v>
+      </c>
+      <c r="M133">
+        <v>106.6925344</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -8632,8 +9461,14 @@
       <c r="J134">
         <v>4</v>
       </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L134">
+        <v>10.89064260000001</v>
+      </c>
+      <c r="M134">
+        <v>106.6622703</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -8664,8 +9499,14 @@
       <c r="J135">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L135">
+        <v>10.869593000000011</v>
+      </c>
+      <c r="M135">
+        <v>106.64793589999999</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -8696,8 +9537,14 @@
       <c r="J136">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L136">
+        <v>10.86293319999997</v>
+      </c>
+      <c r="M136">
+        <v>106.631809</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -8728,8 +9575,14 @@
       <c r="J137">
         <v>4</v>
       </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L137">
+        <v>10.8349841</v>
+      </c>
+      <c r="M137">
+        <v>106.6582322</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -8760,8 +9613,14 @@
       <c r="J138">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L138">
+        <v>10.8231406</v>
+      </c>
+      <c r="M138">
+        <v>106.6934509</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -8792,8 +9651,14 @@
       <c r="J139">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L139">
+        <v>10.829236400000021</v>
+      </c>
+      <c r="M139">
+        <v>106.6726621</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -8824,8 +9689,14 @@
       <c r="J140">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L140">
+        <v>10.84034919999999</v>
+      </c>
+      <c r="M140">
+        <v>106.68306010000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -8856,8 +9727,14 @@
       <c r="J141">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L141">
+        <v>10.84189599999999</v>
+      </c>
+      <c r="M141">
+        <v>106.65614600000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -8888,8 +9765,14 @@
       <c r="J142">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L142">
+        <v>10.83619639999999</v>
+      </c>
+      <c r="M142">
+        <v>106.6710243</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -8920,8 +9803,14 @@
       <c r="J143">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L143">
+        <v>10.83300199999999</v>
+      </c>
+      <c r="M143">
+        <v>106.6912603</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -8952,8 +9841,14 @@
       <c r="J144">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L144">
+        <v>10.831755199999989</v>
+      </c>
+      <c r="M144">
+        <v>106.67407799999999</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -8984,8 +9879,14 @@
       <c r="J145">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L145">
+        <v>10.834860900000001</v>
+      </c>
+      <c r="M145">
+        <v>106.6671607</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
@@ -9016,8 +9917,14 @@
       <c r="J146">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L146">
+        <v>10.823678499999991</v>
+      </c>
+      <c r="M146">
+        <v>106.6762533</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
@@ -9048,8 +9955,14 @@
       <c r="J147">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L147">
+        <v>10.786305799999999</v>
+      </c>
+      <c r="M147">
+        <v>106.6814598</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
@@ -9080,8 +9993,14 @@
       <c r="J148">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L148">
+        <v>10.79629130000002</v>
+      </c>
+      <c r="M148">
+        <v>106.6876742</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
@@ -9112,8 +10031,14 @@
       <c r="J149">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L149">
+        <v>10.79581769999997</v>
+      </c>
+      <c r="M149">
+        <v>106.68788379999999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
@@ -9144,8 +10069,14 @@
       <c r="J150">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L150">
+        <v>10.800874300000009</v>
+      </c>
+      <c r="M150">
+        <v>106.6688994</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
@@ -9176,8 +10107,14 @@
       <c r="J151">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L151">
+        <v>10.81324390000001</v>
+      </c>
+      <c r="M151">
+        <v>106.6759091</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
@@ -9208,8 +10145,14 @@
       <c r="J152">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L152">
+        <v>10.801496499999971</v>
+      </c>
+      <c r="M152">
+        <v>106.61742529999999</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>152</v>
       </c>
@@ -9240,8 +10183,14 @@
       <c r="J153">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L153">
+        <v>10.76846059999998</v>
+      </c>
+      <c r="M153">
+        <v>106.62718769999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>153</v>
       </c>
@@ -9272,8 +10221,14 @@
       <c r="J154">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L154">
+        <v>10.818384000000011</v>
+      </c>
+      <c r="M154">
+        <v>106.8052448</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>154</v>
       </c>
@@ -9304,8 +10259,14 @@
       <c r="J155">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L155">
+        <v>10.841127199999971</v>
+      </c>
+      <c r="M155">
+        <v>106.823775</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>155</v>
       </c>
@@ -9336,8 +10297,14 @@
       <c r="J156">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L156">
+        <v>10.82090489999999</v>
+      </c>
+      <c r="M156">
+        <v>106.7724387</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>156</v>
       </c>
@@ -9368,8 +10335,14 @@
       <c r="J157">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L157">
+        <v>10.7890259</v>
+      </c>
+      <c r="M157">
+        <v>106.6334537</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>157</v>
       </c>
@@ -9400,8 +10373,14 @@
       <c r="J158">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L158">
+        <v>10.79538390000001</v>
+      </c>
+      <c r="M158">
+        <v>106.66390730000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>158</v>
       </c>
@@ -9432,8 +10411,14 @@
       <c r="J159">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L159">
+        <v>10.7650732</v>
+      </c>
+      <c r="M159">
+        <v>106.665255</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>159</v>
       </c>
@@ -9464,8 +10449,14 @@
       <c r="J160">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L160">
+        <v>10.79593130000001</v>
+      </c>
+      <c r="M160">
+        <v>106.6222138</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
@@ -9496,8 +10487,14 @@
       <c r="J161">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L161">
+        <v>10.77494999999999</v>
+      </c>
+      <c r="M161">
+        <v>106.6438903</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
@@ -9525,8 +10522,14 @@
       <c r="J162">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L162">
+        <v>10.80104360000003</v>
+      </c>
+      <c r="M162">
+        <v>106.6650508</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
@@ -9557,8 +10560,14 @@
       <c r="J163">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L163">
+        <v>10.794494899999989</v>
+      </c>
+      <c r="M163">
+        <v>106.6647297</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
@@ -9589,8 +10598,14 @@
       <c r="J164">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L164">
+        <v>10.80508289999999</v>
+      </c>
+      <c r="M164">
+        <v>106.6686603</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
@@ -9621,8 +10636,14 @@
       <c r="J165">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L165">
+        <v>10.81305560000002</v>
+      </c>
+      <c r="M165">
+        <v>106.6655556</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
@@ -9653,8 +10674,14 @@
       <c r="J166">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L166">
+        <v>10.7966219</v>
+      </c>
+      <c r="M166">
+        <v>106.6674769</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
@@ -9685,8 +10712,14 @@
       <c r="J167">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L167">
+        <v>10.778707099999981</v>
+      </c>
+      <c r="M167">
+        <v>106.64919140000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
@@ -9714,8 +10747,14 @@
       <c r="J168">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L168">
+        <v>10.77461569999998</v>
+      </c>
+      <c r="M168">
+        <v>106.6530185</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
@@ -9746,8 +10785,14 @@
       <c r="J169">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L169">
+        <v>10.805262999999981</v>
+      </c>
+      <c r="M169">
+        <v>106.6606578</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
@@ -9778,8 +10823,14 @@
       <c r="J170">
         <v>4</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L170">
+        <v>10.800602599999991</v>
+      </c>
+      <c r="M170">
+        <v>106.6582188</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
@@ -9810,8 +10861,14 @@
       <c r="J171">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L171">
+        <v>10.800004800000011</v>
+      </c>
+      <c r="M171">
+        <v>106.6661782</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
@@ -9842,8 +10899,14 @@
       <c r="J172">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L172">
+        <v>10.79316549999999</v>
+      </c>
+      <c r="M172">
+        <v>106.6660782</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
@@ -9874,8 +10937,14 @@
       <c r="J173">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L173">
+        <v>10.796485899999981</v>
+      </c>
+      <c r="M173">
+        <v>106.64764629999991</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
@@ -9906,8 +10975,14 @@
       <c r="J174">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L174">
+        <v>10.79651630000002</v>
+      </c>
+      <c r="M174">
+        <v>106.68846499999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
@@ -9938,8 +11013,14 @@
       <c r="J175">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L175">
+        <v>10.789755100000029</v>
+      </c>
+      <c r="M175">
+        <v>106.6610082</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
@@ -9970,8 +11051,14 @@
       <c r="J176">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L176">
+        <v>10.78839389999999</v>
+      </c>
+      <c r="M176">
+        <v>106.6428423</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>176</v>
       </c>
@@ -10002,8 +11089,14 @@
       <c r="J177">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L177">
+        <v>10.74274969999999</v>
+      </c>
+      <c r="M177">
+        <v>106.6119309</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>177</v>
       </c>
@@ -10034,8 +11127,14 @@
       <c r="J178">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L178">
+        <v>10.80635940000001</v>
+      </c>
+      <c r="M178">
+        <v>106.6077293</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>178</v>
       </c>
@@ -10066,8 +11165,14 @@
       <c r="J179">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L179">
+        <v>10.84904449999998</v>
+      </c>
+      <c r="M179">
+        <v>106.75966510000001</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
@@ -10098,8 +11203,14 @@
       <c r="J180">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L180">
+        <v>10.75515399999999</v>
+      </c>
+      <c r="M180">
+        <v>106.5712774</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
@@ -10130,8 +11241,14 @@
       <c r="J181">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L181">
+        <v>10.7429025</v>
+      </c>
+      <c r="M181">
+        <v>106.612285</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
@@ -10162,8 +11279,14 @@
       <c r="J182">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L182">
+        <v>10.846431599999971</v>
+      </c>
+      <c r="M182">
+        <v>106.7985201</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
@@ -10194,8 +11317,14 @@
       <c r="J183">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L183">
+        <v>10.73149789999999</v>
+      </c>
+      <c r="M183">
+        <v>106.6098408</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
@@ -10226,8 +11355,14 @@
       <c r="J184">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L184">
+        <v>10.728880100000019</v>
+      </c>
+      <c r="M184">
+        <v>106.61971339999999</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>184</v>
       </c>
@@ -10258,8 +11393,14 @@
       <c r="J185">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L185">
+        <v>10.73033690000001</v>
+      </c>
+      <c r="M185">
+        <v>106.6038563</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>185</v>
       </c>
@@ -10290,8 +11431,14 @@
       <c r="J186">
         <v>4</v>
       </c>
-    </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L186">
+        <v>10.74207619999998</v>
+      </c>
+      <c r="M186">
+        <v>106.6199974</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>186</v>
       </c>
@@ -10325,8 +11472,14 @@
       <c r="K187" s="1" t="s">
         <v>1070</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L187">
+        <v>10.7796599</v>
+      </c>
+      <c r="M187">
+        <v>106.5135875</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>187</v>
       </c>
@@ -10360,8 +11513,14 @@
       <c r="K188" s="1" t="s">
         <v>1078</v>
       </c>
-    </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L188">
+        <v>10.80319549999998</v>
+      </c>
+      <c r="M188">
+        <v>106.70117430000001</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>188</v>
       </c>
@@ -10395,8 +11554,14 @@
       <c r="K189" s="1" t="s">
         <v>1085</v>
       </c>
-    </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L189">
+        <v>10.67102929999999</v>
+      </c>
+      <c r="M189">
+        <v>106.6457733</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>189</v>
       </c>
@@ -10430,8 +11595,14 @@
       <c r="K190" s="1" t="s">
         <v>1089</v>
       </c>
-    </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L190">
+        <v>10.721287699999991</v>
+      </c>
+      <c r="M190">
+        <v>106.536269</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>190</v>
       </c>
@@ -10465,8 +11636,14 @@
       <c r="K191" s="1" t="s">
         <v>1095</v>
       </c>
-    </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L191">
+        <v>10.731219500000011</v>
+      </c>
+      <c r="M191">
+        <v>106.67314260000001</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>191</v>
       </c>
@@ -10500,8 +11677,14 @@
       <c r="K192" s="1" t="s">
         <v>1101</v>
       </c>
-    </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L192">
+        <v>10.72533269999999</v>
+      </c>
+      <c r="M192">
+        <v>106.6747058</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>192</v>
       </c>
@@ -10535,8 +11718,14 @@
       <c r="K193" s="1" t="s">
         <v>1107</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L193">
+        <v>10.92012190000001</v>
+      </c>
+      <c r="M193">
+        <v>106.6830688</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>193</v>
       </c>
@@ -10570,8 +11759,14 @@
       <c r="K194" s="1" t="s">
         <v>1113</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L194">
+        <v>10.76979349999999</v>
+      </c>
+      <c r="M194">
+        <v>106.52654990000001</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>194</v>
       </c>
@@ -10605,8 +11800,14 @@
       <c r="K195" s="1" t="s">
         <v>1120</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L195">
+        <v>10.42037719999999</v>
+      </c>
+      <c r="M195">
+        <v>106.9591958</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>195</v>
       </c>
@@ -10640,8 +11841,14 @@
       <c r="K196" s="1" t="s">
         <v>1127</v>
       </c>
-    </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L196">
+        <v>10.377776400000011</v>
+      </c>
+      <c r="M196">
+        <v>106.89097599999999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>196</v>
       </c>
@@ -10675,8 +11882,14 @@
       <c r="K197" s="1" t="s">
         <v>1132</v>
       </c>
-    </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L197">
+        <v>10.38694680000002</v>
+      </c>
+      <c r="M197">
+        <v>106.9193279</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>197</v>
       </c>
@@ -10710,8 +11923,14 @@
       <c r="K198" s="1" t="s">
         <v>1139</v>
       </c>
-    </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L198">
+        <v>10.385631499999979</v>
+      </c>
+      <c r="M198">
+        <v>106.9214867</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>198</v>
       </c>
@@ -10745,8 +11964,14 @@
       <c r="K199" s="1" t="s">
         <v>1146</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L199">
+        <v>12.35967500000001</v>
+      </c>
+      <c r="M199">
+        <v>109.21290999999999</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>199</v>
       </c>
@@ -10780,8 +12005,14 @@
       <c r="K200" s="1" t="s">
         <v>1153</v>
       </c>
-    </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L200">
+        <v>10.48961410000002</v>
+      </c>
+      <c r="M200">
+        <v>106.7956002</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>200</v>
       </c>
@@ -10812,8 +12043,14 @@
       <c r="K201" s="1" t="s">
         <v>1160</v>
       </c>
-    </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L201">
+        <v>10.810360100000009</v>
+      </c>
+      <c r="M201">
+        <v>106.7089454</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>201</v>
       </c>
@@ -10847,8 +12084,14 @@
       <c r="K202" s="1" t="s">
         <v>1167</v>
       </c>
-    </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L202">
+        <v>10.744099</v>
+      </c>
+      <c r="M202">
+        <v>106.72960860000001</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>202</v>
       </c>
@@ -10882,8 +12125,14 @@
       <c r="K203" s="1" t="s">
         <v>1174</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L203">
+        <v>10.84430570000001</v>
+      </c>
+      <c r="M203">
+        <v>106.77934810000001</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>203</v>
       </c>
@@ -10914,8 +12163,14 @@
       <c r="J204">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L204">
+        <v>10.829624600000001</v>
+      </c>
+      <c r="M204">
+        <v>106.6926802</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>204</v>
       </c>
@@ -10949,8 +12204,14 @@
       <c r="K205" s="1" t="s">
         <v>1185</v>
       </c>
-    </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L205">
+        <v>10.697900400000011</v>
+      </c>
+      <c r="M205">
+        <v>106.73893630000001</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>205</v>
       </c>
@@ -10984,8 +12245,14 @@
       <c r="K206" s="1" t="s">
         <v>1189</v>
       </c>
-    </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L206">
+        <v>10.84343519999997</v>
+      </c>
+      <c r="M206">
+        <v>106.7888933</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>206</v>
       </c>
@@ -11019,8 +12286,14 @@
       <c r="K207" s="1" t="s">
         <v>1196</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L207">
+        <v>10.645601900000001</v>
+      </c>
+      <c r="M207">
+        <v>106.73168149999999</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>207</v>
       </c>
@@ -11054,8 +12327,14 @@
       <c r="K208" s="1" t="s">
         <v>1202</v>
       </c>
-    </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L208">
+        <v>10.90916889999999</v>
+      </c>
+      <c r="M208">
+        <v>106.64654470000001</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>208</v>
       </c>
@@ -11089,8 +12368,14 @@
       <c r="K209" s="1" t="s">
         <v>1210</v>
       </c>
-    </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L209">
+        <v>10.91750789999999</v>
+      </c>
+      <c r="M209">
+        <v>106.6521915</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>209</v>
       </c>
@@ -11124,8 +12409,14 @@
       <c r="K210" s="1" t="s">
         <v>1215</v>
       </c>
-    </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L210">
+        <v>10.86822500000001</v>
+      </c>
+      <c r="M210">
+        <v>106.55854290000001</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>210</v>
       </c>
@@ -11159,8 +12450,14 @@
       <c r="K211" s="1" t="s">
         <v>1222</v>
       </c>
-    </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L211">
+        <v>10.85935180000001</v>
+      </c>
+      <c r="M211">
+        <v>106.5851098</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>211</v>
       </c>
@@ -11194,8 +12491,14 @@
       <c r="K212" s="1" t="s">
         <v>1229</v>
       </c>
-    </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L212">
+        <v>10.92012190000001</v>
+      </c>
+      <c r="M212">
+        <v>106.6830688</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>212</v>
       </c>
@@ -11229,8 +12532,14 @@
       <c r="K213" s="1" t="s">
         <v>1235</v>
       </c>
-    </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L213">
+        <v>10.88915729999998</v>
+      </c>
+      <c r="M213">
+        <v>106.59518370000001</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>213</v>
       </c>
@@ -11264,8 +12573,14 @@
       <c r="K214" s="1" t="s">
         <v>1241</v>
       </c>
-    </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L214">
+        <v>10.831987900000019</v>
+      </c>
+      <c r="M214">
+        <v>106.6215814</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214</v>
       </c>
@@ -11299,8 +12614,14 @@
       <c r="K215" s="1" t="s">
         <v>1247</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L215">
+        <v>10.885567600000011</v>
+      </c>
+      <c r="M215">
+        <v>106.6016176</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>215</v>
       </c>
@@ -11334,8 +12655,14 @@
       <c r="K216" s="1" t="s">
         <v>1253</v>
       </c>
-    </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L216">
+        <v>10.900282099999981</v>
+      </c>
+      <c r="M216">
+        <v>106.5818117</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>216</v>
       </c>
@@ -11366,8 +12693,14 @@
       <c r="K217" s="1" t="s">
         <v>1260</v>
       </c>
-    </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L217">
+        <v>10.883212300000009</v>
+      </c>
+      <c r="M217">
+        <v>106.6039631</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>217</v>
       </c>
@@ -11401,8 +12734,14 @@
       <c r="K218" s="1" t="s">
         <v>1267</v>
       </c>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L218">
+        <v>11.14159100000002</v>
+      </c>
+      <c r="M218">
+        <v>106.4615963</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>218</v>
       </c>
@@ -11436,8 +12775,14 @@
       <c r="K219" s="1" t="s">
         <v>1273</v>
       </c>
-    </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L219">
+        <v>11.1463889</v>
+      </c>
+      <c r="M219">
+        <v>106.4594444</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>219</v>
       </c>
@@ -11471,8 +12816,14 @@
       <c r="K220" s="1" t="s">
         <v>1280</v>
       </c>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L220">
+        <v>11.1084397</v>
+      </c>
+      <c r="M220">
+        <v>106.51857029999999</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>220</v>
       </c>
@@ -11506,8 +12857,14 @@
       <c r="K221" t="s">
         <v>1286</v>
       </c>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L221">
+        <v>11.1302805</v>
+      </c>
+      <c r="M221">
+        <v>106.5028338</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>221</v>
       </c>
@@ -11541,8 +12898,14 @@
       <c r="K222" s="1" t="s">
         <v>1292</v>
       </c>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L222">
+        <v>10.9395115</v>
+      </c>
+      <c r="M222">
+        <v>106.54996250000001</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>222</v>
       </c>
@@ -11573,8 +12936,14 @@
       <c r="K223" s="1" t="s">
         <v>1298</v>
       </c>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L223">
+        <v>11.062424</v>
+      </c>
+      <c r="M223">
+        <v>106.4883342</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>223</v>
       </c>
@@ -11604,6 +12973,12 @@
       </c>
       <c r="K224" s="1" t="s">
         <v>1303</v>
+      </c>
+      <c r="L224">
+        <v>11.064323399999999</v>
+      </c>
+      <c r="M224">
+        <v>106.4842494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>